<commit_message>
Change to Excel for sprint 2 stories
</commit_message>
<xml_diff>
--- a/TeamANSReport.xlsx
+++ b/TeamANSReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\Current Sem\Agile\Project\SSW-555-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457D5DA3-A845-40A1-A9A2-9E92131BB058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="549" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="549" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -30,20 +31,19 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="200">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -670,12 +670,15 @@
   </si>
   <si>
     <t>Coding</t>
+  </si>
+  <si>
+    <t>SK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -814,7 +817,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -843,6 +846,7 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="65"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1997,19 +2001,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2089,14 +2093,14 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
@@ -2104,20 +2108,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="42.75" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2241,6 +2245,40 @@
         <v>175</v>
       </c>
       <c r="E9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2252,21 +2290,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2446,21 +2484,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2506,14 +2544,14 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>983</v>
       </c>
       <c r="E3">
         <v>120</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>491.5</v>
       </c>
     </row>
   </sheetData>
@@ -2525,23 +2563,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
-    <col min="7" max="7" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2756,7 +2794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>194</v>
       </c>
@@ -2779,16 +2817,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B2" sqref="B2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2815,6 +2853,46 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="18">
+        <v>50</v>
+      </c>
+      <c r="F2" s="18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="18">
+        <v>80</v>
+      </c>
+      <c r="F3" s="18">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2825,16 +2903,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2870,16 +2948,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2915,17 +2993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2939,7 +3017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -2950,7 +3028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -2961,7 +3039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -2972,7 +3050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2983,7 +3061,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -2994,7 +3072,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -3005,7 +3083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -3016,7 +3094,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -3027,7 +3105,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -3038,7 +3116,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -3049,7 +3127,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -3060,7 +3138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -3071,7 +3149,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>125</v>
       </c>
@@ -3082,7 +3160,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -3093,7 +3171,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -3104,7 +3182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -3115,7 +3193,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -3126,7 +3204,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>130</v>
       </c>
@@ -3137,7 +3215,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -3148,7 +3226,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -3159,7 +3237,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -3170,7 +3248,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>134</v>
       </c>
@@ -3181,7 +3259,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -3192,7 +3270,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -3203,7 +3281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -3214,7 +3292,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -3225,7 +3303,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -3236,7 +3314,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -3247,7 +3325,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -3258,7 +3336,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -3269,7 +3347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -3280,7 +3358,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -3291,7 +3369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -3302,7 +3380,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -3313,7 +3391,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -3324,7 +3402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -3335,7 +3413,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -3346,7 +3424,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -3357,7 +3435,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -3368,7 +3446,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -3379,7 +3457,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>153</v>
       </c>
@@ -3390,7 +3468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
Sprint 3 Stories updated
</commit_message>
<xml_diff>
--- a/TeamANSReport.xlsx
+++ b/TeamANSReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Stevens\555\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stevens\Current Sem\Agile\Project\SSW-555-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37A9E6F-B844-4FCD-8B0A-327FB2E03810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" tabRatio="549" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="549" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="201">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -672,12 +673,15 @@
   </si>
   <si>
     <t>NP</t>
+  </si>
+  <si>
+    <t>Changing main parser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -725,7 +729,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,6 +745,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,7 +832,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -853,6 +863,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1104,7 +1115,7 @@
                   <c:v>02-21-2022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7/3</c:v>
+                  <c:v>7-3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2007,19 +2018,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2099,14 +2110,14 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
@@ -2114,20 +2125,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="42.75" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2364,21 +2375,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2558,21 +2569,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2626,23 +2637,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
-    <col min="7" max="7" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2875,7 +2886,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>192</v>
       </c>
@@ -2898,19 +2909,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2939,7 +2950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>113</v>
       </c>
@@ -2968,7 +2979,7 @@
         <v>43184</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>116</v>
       </c>
@@ -2997,7 +3008,7 @@
         <v>43184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>130</v>
       </c>
@@ -3026,7 +3037,7 @@
         <v>43186</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>129</v>
       </c>
@@ -3055,7 +3066,7 @@
         <v>43186</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -3084,7 +3095,7 @@
         <v>43184</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3111,6 +3122,40 @@
       </c>
       <c r="I9" s="13">
         <v>43184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3121,16 +3166,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3157,6 +3206,46 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3166,16 +3255,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3211,17 +3300,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3235,7 +3324,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>113</v>
       </c>
@@ -3246,7 +3335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>114</v>
       </c>
@@ -3257,7 +3346,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>115</v>
       </c>
@@ -3268,7 +3357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>116</v>
       </c>
@@ -3279,7 +3368,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>117</v>
       </c>
@@ -3290,7 +3379,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>118</v>
       </c>
@@ -3301,7 +3390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>119</v>
       </c>
@@ -3312,7 +3401,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>120</v>
       </c>
@@ -3323,7 +3412,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>121</v>
       </c>
@@ -3334,7 +3423,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>122</v>
       </c>
@@ -3345,8 +3434,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B12" t="s">
@@ -3356,8 +3445,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>124</v>
       </c>
       <c r="B13" t="s">
@@ -3367,7 +3456,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>125</v>
       </c>
@@ -3378,7 +3467,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -3389,7 +3478,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -3400,7 +3489,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -3411,8 +3500,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B18" t="s">
@@ -3422,8 +3511,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B19" t="s">
@@ -3433,7 +3522,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -3444,7 +3533,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -3455,7 +3544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -3466,7 +3555,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>134</v>
       </c>
@@ -3477,7 +3566,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -3488,7 +3577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -3499,7 +3588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -3510,7 +3599,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -3521,7 +3610,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -3532,7 +3621,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -3543,7 +3632,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -3554,7 +3643,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -3565,7 +3654,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -3576,7 +3665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -3587,7 +3676,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -3598,7 +3687,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -3609,7 +3698,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -3620,7 +3709,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -3631,7 +3720,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -3642,7 +3731,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -3653,7 +3742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -3664,7 +3753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -3675,7 +3764,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>153</v>
       </c>
@@ -3686,7 +3775,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
Added Sprint 4 User Stories for AA
</commit_message>
<xml_diff>
--- a/TeamANSReport.xlsx
+++ b/TeamANSReport.xlsx
@@ -3565,7 +3565,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3573,7 +3573,7 @@
     <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3613,13 +3613,22 @@
         <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2">
         <v>30</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="13">
+        <v>43209</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>